<commit_message>
Message Log tests + some improvements
</commit_message>
<xml_diff>
--- a/Domibus-MSH-selenium-ui-tests/TestCase_Domibus-4.1.xlsx
+++ b/Domibus-MSH-selenium-ui-tests/TestCase_Domibus-4.1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="798">
   <si>
     <t xml:space="preserve">Step</t>
   </si>
@@ -215,6 +215,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Messages are available for download only on the </t>
     </r>
@@ -224,6 +225,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">receiver</t>
     </r>
@@ -233,6 +235,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> node or on the sending node if message was not sent (status = WAITING_FOR_RETRY or SEND_FAILURE)
 Message must still have it's payload (the payload has not been deleted from the message)
@@ -244,6 +247,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">containing</t>
     </r>
@@ -253,6 +257,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">:
 - the message payload
@@ -419,6 +424,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Modal with form allowing the user to create a filter opens
 User can choose only plugins configured for his </t>
@@ -429,6 +435,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">select</t>
     </r>
@@ -438,6 +445,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> domain
 After user enters required data and presses OK the Save and Cancel buttons become active</t>
@@ -550,6 +558,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">User is prompted if he wishes to Cancel the changes. If user presses Yes he is taken to the </t>
     </r>
@@ -559,6 +568,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">corresponding</t>
     </r>
@@ -568,6 +578,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> domains Message filters page.
 If user chooses Not then the domain doesn't change allowing the user to save his changes.</t>
@@ -830,6 +841,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Modal with </t>
     </r>
@@ -839,6 +851,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">possible</t>
     </r>
@@ -848,6 +861,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> destinations opens allowing the user to cancel or confirm the action
 If the user confirms the message is moved to the selected destination queue. Else the message is not moved</t>
@@ -860,6 +874,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">List of messages is refreshed
 Only messages </t>
@@ -870,6 +885,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">corresponding</t>
     </r>
@@ -879,6 +895,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> to the new domain are shown
 List is at page 1</t>
@@ -1114,6 +1131,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Confirmation modal appears.
 List </t>
@@ -1124,6 +1142,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">is</t>
     </r>
@@ -1133,6 +1152,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> refreshed and user reappears.
 Save and Cancel buttons become disabled again
@@ -1149,6 +1169,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Confirmation modal appears.
 List </t>
@@ -1159,6 +1180,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">is</t>
     </r>
@@ -1168,6 +1190,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> refreshed and user is deleted permanently
 Save and Cancel buttons become disabled again
@@ -1345,6 +1368,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"Filter area has the following filters:
 - </t>
@@ -1355,6 +1379,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Authentication</t>
     </r>
@@ -1364,6 +1389,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> type
 - User role
@@ -1377,6 +1403,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Authentication</t>
     </r>
@@ -1386,6 +1413,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> type dropdown has preselected the BASIC value.
 All other filters are empty.
@@ -1400,6 +1428,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1410,6 +1439,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Grid shows only columns:
 - Username
@@ -1424,6 +1454,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">disabled</t>
     </r>
@@ -1433,6 +1464,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> except New button.
 </t>
@@ -1453,6 +1485,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Confirmation modal appears.
 List </t>
@@ -1463,6 +1496,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">is</t>
     </r>
@@ -1472,6 +1506,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> refreshed and user is deleted </t>
     </r>
@@ -1481,6 +1516,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">permanently.
 </t>
@@ -1491,6 +1527,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Save and Cancel buttons become disabled again
 </t>
@@ -1852,6 +1889,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">User is presented with dropdown allowing him to pick the party ID
 Test and Update buttons are present and disabled.
@@ -1865,6 +1903,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">initially</t>
     </r>
@@ -1874,6 +1913,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> don't contain any information and are not editable</t>
     </r>
@@ -1909,6 +1949,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">The submit test message form now contains 3 fields:
 Final recipient
@@ -1925,6 +1966,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">initially</t>
     </r>
@@ -1934,6 +1976,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> don't contain any information and are not editable</t>
     </r>
@@ -1966,6 +2009,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">File is visible in the PMode - Current page
 Changes take effect </t>
@@ -1976,6 +2020,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">immediately.
 </t>
@@ -1986,6 +2031,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">New row is added to the Archive table with link to the current file</t>
     </r>
@@ -2093,6 +2139,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Modal opens allowing the user to enter the </t>
     </r>
@@ -2102,6 +2149,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">necessary</t>
     </r>
@@ -2111,6 +2159,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> data to define a new party.
 Required information is clearly defined.
@@ -2122,6 +2171,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">effect</t>
     </r>
@@ -2131,6 +2181,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2140,6 +2191,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">immediately.</t>
     </r>
@@ -2154,6 +2206,7 @@
         <color rgb="FF000000"/>
         <rFont val="Verdana"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Modal opens allowing the user to enter the </t>
     </r>
@@ -2163,6 +2216,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">necessary</t>
     </r>
@@ -2172,6 +2226,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> data to edit the party.
 Required information is clearly defined.
@@ -2183,6 +2238,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">effect</t>
     </r>
@@ -2192,6 +2248,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2201,6 +2258,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">immediately.</t>
     </r>
@@ -3296,6 +3354,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3313,29 +3372,64 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="18"/>
+      <b val="true"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -3343,6 +3437,81 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -3350,133 +3519,49 @@
       <color rgb="FF0000EE"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3484,18 +3569,21 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -3503,18 +3591,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -3523,30 +3614,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -3564,6 +3631,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -3648,128 +3739,128 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="8" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="8" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="5" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="28">
@@ -3781,27 +3872,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="9" borderId="0" xfId="50" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="9" borderId="0" xfId="46" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="9" borderId="0" xfId="50" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="9" borderId="0" xfId="46" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="9" borderId="0" xfId="50" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="9" borderId="0" xfId="46" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="50" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="46" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="10" borderId="0" xfId="50" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="10" borderId="0" xfId="46" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="50" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="46" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3813,7 +3904,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="50" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="46" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3825,7 +3916,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="9" borderId="0" xfId="50" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="9" borderId="0" xfId="46" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3877,7 +3968,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="48" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3893,41 +3984,41 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
-    <cellStyle name="Accent 1 5" xfId="37"/>
-    <cellStyle name="Accent 2 6" xfId="38"/>
-    <cellStyle name="Accent 3 7" xfId="39"/>
-    <cellStyle name="Accent 4" xfId="40"/>
-    <cellStyle name="Bad 2" xfId="41"/>
-    <cellStyle name="Error 8" xfId="42"/>
-    <cellStyle name="Footnote 9" xfId="43"/>
-    <cellStyle name="Good 2" xfId="44"/>
-    <cellStyle name="Heading 1 2" xfId="45"/>
-    <cellStyle name="Heading 10" xfId="46"/>
-    <cellStyle name="Heading 2 2" xfId="47"/>
-    <cellStyle name="Hyperlink 11" xfId="48"/>
-    <cellStyle name="Neutral 2" xfId="49"/>
-    <cellStyle name="Normal 2" xfId="50"/>
-    <cellStyle name="Note 2" xfId="51"/>
-    <cellStyle name="Status 12" xfId="52"/>
-    <cellStyle name="Text 13" xfId="53"/>
-    <cellStyle name="Warning 14" xfId="54"/>
+    <cellStyle name="Accent 1 18" xfId="20"/>
+    <cellStyle name="Accent 1 5" xfId="21"/>
+    <cellStyle name="Accent 17" xfId="22"/>
+    <cellStyle name="Accent 2 19" xfId="23"/>
+    <cellStyle name="Accent 2 6" xfId="24"/>
+    <cellStyle name="Accent 3 20" xfId="25"/>
+    <cellStyle name="Accent 3 7" xfId="26"/>
+    <cellStyle name="Accent 4" xfId="27"/>
+    <cellStyle name="Bad 13" xfId="28"/>
+    <cellStyle name="Bad 2" xfId="29"/>
+    <cellStyle name="Error 16" xfId="30"/>
+    <cellStyle name="Error 8" xfId="31"/>
+    <cellStyle name="Footnote 8" xfId="32"/>
+    <cellStyle name="Footnote 9" xfId="33"/>
+    <cellStyle name="Good 11" xfId="34"/>
+    <cellStyle name="Good 2" xfId="35"/>
+    <cellStyle name="Heading 1 2" xfId="36"/>
+    <cellStyle name="Heading 1 4" xfId="37"/>
+    <cellStyle name="Heading 10" xfId="38"/>
+    <cellStyle name="Heading 2 2" xfId="39"/>
+    <cellStyle name="Heading 2 5" xfId="40"/>
+    <cellStyle name="Heading 3" xfId="41"/>
+    <cellStyle name="Hyperlink 11" xfId="42"/>
+    <cellStyle name="Hyperlink 9" xfId="43"/>
+    <cellStyle name="Neutral 12" xfId="44"/>
+    <cellStyle name="Neutral 2" xfId="45"/>
+    <cellStyle name="Normal 2" xfId="46"/>
+    <cellStyle name="Note 2" xfId="47"/>
+    <cellStyle name="Note 7" xfId="48"/>
+    <cellStyle name="Status 10" xfId="49"/>
+    <cellStyle name="Status 12" xfId="50"/>
+    <cellStyle name="Text 13" xfId="51"/>
+    <cellStyle name="Text 6" xfId="52"/>
+    <cellStyle name="Warning 14" xfId="53"/>
+    <cellStyle name="Warning 15" xfId="54"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3999,8 +4090,8 @@
   </sheetPr>
   <dimension ref="A1:D351"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4011,7 +4102,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4023,7 +4114,7 @@
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -4031,7 +4122,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -4043,7 +4134,7 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -4055,7 +4146,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -4067,7 +4158,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -4079,7 +4170,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -4091,7 +4182,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="n">
@@ -4099,7 +4190,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -4107,7 +4198,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -4119,7 +4210,7 @@
       </c>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -4131,7 +4222,7 @@
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -4143,7 +4234,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -4155,7 +4246,7 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -4167,7 +4258,7 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="n">
@@ -4175,7 +4266,7 @@
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -4183,7 +4274,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="181.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -4195,7 +4286,7 @@
       </c>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
@@ -4207,7 +4298,7 @@
       </c>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
@@ -4233,7 +4324,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -4245,7 +4336,7 @@
       </c>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
@@ -4257,74 +4348,88 @@
       </c>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="192" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="76.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4334,7 +4439,9 @@
       <c r="B30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4344,17 +4451,21 @@
       <c r="B31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5" t="n">
+        <v>1</v>
+      </c>
       <c r="D32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4407,7 +4518,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>64</v>
       </c>
@@ -4417,7 +4528,7 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
         <v>66</v>
       </c>
@@ -4427,7 +4538,7 @@
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
         <v>68</v>
       </c>
@@ -4437,7 +4548,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
         <v>70</v>
       </c>
@@ -4447,7 +4558,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
         <v>72</v>
       </c>
@@ -4457,7 +4568,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
         <v>74</v>
       </c>
@@ -4467,7 +4578,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
         <v>76</v>
       </c>
@@ -4477,7 +4588,7 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
         <v>78</v>
       </c>
@@ -4497,7 +4608,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
         <v>82</v>
       </c>
@@ -4507,7 +4618,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>84</v>
       </c>
@@ -4515,7 +4626,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
         <v>85</v>
       </c>
@@ -4527,7 +4638,7 @@
       </c>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
         <v>87</v>
       </c>
@@ -4539,7 +4650,7 @@
       </c>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
         <v>89</v>
       </c>
@@ -4551,7 +4662,7 @@
       </c>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
         <v>91</v>
       </c>
@@ -4563,7 +4674,7 @@
       </c>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="7" t="s">
         <v>93</v>
       </c>
@@ -4575,7 +4686,7 @@
       </c>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
         <v>89</v>
       </c>
@@ -4587,7 +4698,7 @@
       </c>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
         <v>96</v>
       </c>
@@ -4599,7 +4710,7 @@
       </c>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
         <v>98</v>
       </c>
@@ -4611,7 +4722,7 @@
       </c>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
         <v>100</v>
       </c>
@@ -4623,7 +4734,7 @@
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="69.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7" t="s">
         <v>102</v>
       </c>
@@ -4635,7 +4746,7 @@
       </c>
       <c r="D58" s="5"/>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
         <v>104</v>
       </c>
@@ -4647,7 +4758,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
         <v>106</v>
       </c>
@@ -4657,7 +4768,7 @@
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
         <v>89</v>
       </c>
@@ -4667,7 +4778,7 @@
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5" t="s">
         <v>108</v>
       </c>
@@ -4677,7 +4788,7 @@
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
         <v>109</v>
       </c>
@@ -4687,7 +4798,7 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
         <v>89</v>
       </c>
@@ -4697,7 +4808,7 @@
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
         <v>112</v>
       </c>
@@ -4707,7 +4818,7 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
         <v>114</v>
       </c>
@@ -4717,7 +4828,7 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
         <v>116</v>
       </c>
@@ -4727,7 +4838,7 @@
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
         <v>118</v>
       </c>
@@ -4737,7 +4848,7 @@
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
         <v>120</v>
       </c>
@@ -4747,7 +4858,7 @@
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
     </row>
-    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
         <v>122</v>
       </c>
@@ -4757,7 +4868,7 @@
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
     </row>
-    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
         <v>124</v>
       </c>
@@ -4767,7 +4878,7 @@
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
         <v>126</v>
       </c>
@@ -4777,7 +4888,7 @@
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
         <v>128</v>
       </c>
@@ -4787,7 +4898,7 @@
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
     </row>
-    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
         <v>130</v>
       </c>
@@ -4797,7 +4908,7 @@
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
         <v>132</v>
       </c>
@@ -4807,7 +4918,7 @@
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
     </row>
-    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>133</v>
       </c>
@@ -4817,7 +4928,7 @@
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
         <v>135</v>
       </c>
@@ -4827,7 +4938,7 @@
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
         <v>137</v>
       </c>
@@ -4837,7 +4948,7 @@
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
         <v>80</v>
       </c>
@@ -4847,7 +4958,7 @@
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
         <v>82</v>
       </c>
@@ -4857,7 +4968,7 @@
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
         <v>139</v>
       </c>
@@ -4865,7 +4976,7 @@
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
     </row>
-    <row r="82" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
         <v>140</v>
       </c>
@@ -4877,7 +4988,7 @@
       </c>
       <c r="D82" s="5"/>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
         <v>142</v>
       </c>
@@ -4887,7 +4998,7 @@
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
     </row>
-    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
         <v>144</v>
       </c>
@@ -4899,7 +5010,7 @@
       </c>
       <c r="D84" s="5"/>
     </row>
-    <row r="85" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="125.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5" t="s">
         <v>38</v>
       </c>
@@ -4909,7 +5020,7 @@
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
         <v>147</v>
       </c>
@@ -4919,7 +5030,7 @@
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
         <v>148</v>
       </c>
@@ -4929,7 +5040,7 @@
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
         <v>149</v>
       </c>
@@ -4939,7 +5050,7 @@
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
         <v>151</v>
       </c>
@@ -4949,7 +5060,7 @@
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
         <v>153</v>
       </c>
@@ -4959,7 +5070,7 @@
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
     </row>
-    <row r="91" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
         <v>62</v>
       </c>
@@ -4969,7 +5080,7 @@
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
     </row>
-    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
         <v>64</v>
       </c>
@@ -4979,7 +5090,7 @@
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
         <v>66</v>
       </c>
@@ -4989,7 +5100,7 @@
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
     </row>
-    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
         <v>68</v>
       </c>
@@ -4999,7 +5110,7 @@
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
         <v>70</v>
       </c>
@@ -5009,7 +5120,7 @@
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
     </row>
-    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
         <v>72</v>
       </c>
@@ -5019,7 +5130,7 @@
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
     </row>
-    <row r="97" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
         <v>74</v>
       </c>
@@ -5029,7 +5140,7 @@
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
         <v>159</v>
       </c>
@@ -5039,7 +5150,7 @@
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
         <v>161</v>
       </c>
@@ -5049,7 +5160,7 @@
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
     </row>
-    <row r="100" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
         <v>162</v>
       </c>
@@ -5059,7 +5170,7 @@
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
     </row>
-    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
         <v>164</v>
       </c>
@@ -5069,7 +5180,7 @@
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
         <v>166</v>
       </c>
@@ -5077,7 +5188,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
         <v>168</v>
       </c>
@@ -5085,7 +5196,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
         <v>170</v>
       </c>
@@ -5093,7 +5204,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
         <v>80</v>
       </c>
@@ -5101,7 +5212,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
         <v>82</v>
       </c>
@@ -5109,13 +5220,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="s">
         <v>172</v>
       </c>
       <c r="B107" s="4"/>
     </row>
-    <row r="108" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="236.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
         <v>173</v>
       </c>
@@ -5123,7 +5234,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
         <v>34</v>
       </c>
@@ -5131,7 +5242,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
         <v>176</v>
       </c>
@@ -5139,7 +5250,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
         <v>41</v>
       </c>
@@ -5147,7 +5258,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
         <v>149</v>
       </c>
@@ -5155,7 +5266,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
         <v>45</v>
       </c>
@@ -5163,7 +5274,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="69.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
         <v>177</v>
       </c>
@@ -5171,7 +5282,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
         <v>179</v>
       </c>
@@ -5179,7 +5290,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
         <v>51</v>
       </c>
@@ -5191,7 +5302,7 @@
       <c r="A117" s="5"/>
       <c r="B117" s="5"/>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
         <v>53</v>
       </c>
@@ -5199,7 +5310,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
         <v>55</v>
       </c>
@@ -5207,7 +5318,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
         <v>182</v>
       </c>
@@ -5215,7 +5326,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="5" t="s">
         <v>45</v>
       </c>
@@ -5223,7 +5334,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
         <v>62</v>
       </c>
@@ -5231,7 +5342,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
         <v>64</v>
       </c>
@@ -5239,7 +5350,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
         <v>66</v>
       </c>
@@ -5247,7 +5358,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
         <v>68</v>
       </c>
@@ -5255,7 +5366,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
         <v>186</v>
       </c>
@@ -5263,7 +5374,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
         <v>72</v>
       </c>
@@ -5271,7 +5382,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
         <v>74</v>
       </c>
@@ -5279,7 +5390,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="5" t="s">
         <v>159</v>
       </c>
@@ -5287,7 +5398,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
         <v>189</v>
       </c>
@@ -5295,7 +5406,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
         <v>190</v>
       </c>
@@ -5303,7 +5414,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
         <v>192</v>
       </c>
@@ -5311,7 +5422,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
         <v>194</v>
       </c>
@@ -5319,7 +5430,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
         <v>196</v>
       </c>
@@ -5327,7 +5438,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
         <v>198</v>
       </c>
@@ -5335,7 +5446,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
         <v>199</v>
       </c>
@@ -5343,7 +5454,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="5" t="s">
         <v>80</v>
       </c>
@@ -5351,7 +5462,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
         <v>82</v>
       </c>
@@ -5363,13 +5474,13 @@
       <c r="A139" s="5"/>
       <c r="B139" s="5"/>
     </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="s">
         <v>201</v>
       </c>
       <c r="B140" s="4"/>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
         <v>202</v>
       </c>
@@ -5377,7 +5488,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="7" t="s">
         <v>204</v>
       </c>
@@ -5385,7 +5496,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="5" t="s">
         <v>206</v>
       </c>
@@ -5393,7 +5504,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="5" t="s">
         <v>208</v>
       </c>
@@ -5401,7 +5512,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="5" t="s">
         <v>210</v>
       </c>
@@ -5409,7 +5520,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="s">
         <v>62</v>
       </c>
@@ -5417,7 +5528,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="5" t="s">
         <v>64</v>
       </c>
@@ -5425,7 +5536,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="5" t="s">
         <v>66</v>
       </c>
@@ -5433,7 +5544,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="s">
         <v>68</v>
       </c>
@@ -5441,7 +5552,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="5" t="s">
         <v>72</v>
       </c>
@@ -5449,7 +5560,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="5" t="s">
         <v>74</v>
       </c>
@@ -5457,7 +5568,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="s">
         <v>214</v>
       </c>
@@ -5465,7 +5576,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="5" t="s">
         <v>216</v>
       </c>
@@ -5473,7 +5584,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="s">
         <v>218</v>
       </c>
@@ -5481,7 +5592,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="5" t="s">
         <v>220</v>
       </c>
@@ -5489,7 +5600,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="s">
         <v>80</v>
       </c>
@@ -5497,7 +5608,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="5" t="s">
         <v>82</v>
       </c>
@@ -5505,13 +5616,13 @@
         <v>222</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="4" t="s">
         <v>223</v>
       </c>
       <c r="B158" s="4"/>
     </row>
-    <row r="159" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="5" t="s">
         <v>224</v>
       </c>
@@ -5522,7 +5633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="5" t="s">
         <v>226</v>
       </c>
@@ -5533,7 +5644,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="7" t="s">
         <v>228</v>
       </c>
@@ -5544,7 +5655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="7" t="s">
         <v>230</v>
       </c>
@@ -5555,7 +5666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="7" t="s">
         <v>232</v>
       </c>
@@ -5566,7 +5677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="7" t="s">
         <v>234</v>
       </c>
@@ -5577,7 +5688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="7" t="s">
         <v>236</v>
       </c>
@@ -5588,7 +5699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="7" t="s">
         <v>238</v>
       </c>
@@ -5599,7 +5710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="7" t="s">
         <v>240</v>
       </c>
@@ -5610,7 +5721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="7" t="s">
         <v>242</v>
       </c>
@@ -5621,7 +5732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="5" t="s">
         <v>244</v>
       </c>
@@ -5632,7 +5743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="7" t="s">
         <v>246</v>
       </c>
@@ -5643,7 +5754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="7" t="s">
         <v>248</v>
       </c>
@@ -5654,7 +5765,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="5" t="s">
         <v>250</v>
       </c>
@@ -5665,7 +5776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="5" t="s">
         <v>252</v>
       </c>
@@ -5676,7 +5787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="5" t="s">
         <v>254</v>
       </c>
@@ -5687,7 +5798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="5" t="s">
         <v>256</v>
       </c>
@@ -5698,7 +5809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="5" t="s">
         <v>258</v>
       </c>
@@ -5709,7 +5820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="5" t="s">
         <v>260</v>
       </c>
@@ -5720,7 +5831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="5" t="s">
         <v>262</v>
       </c>
@@ -5731,7 +5842,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="5" t="s">
         <v>264</v>
       </c>
@@ -5742,7 +5853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="5" t="s">
         <v>266</v>
       </c>
@@ -5753,7 +5864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="5" t="s">
         <v>267</v>
       </c>
@@ -5764,7 +5875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="5" t="s">
         <v>268</v>
       </c>
@@ -5775,7 +5886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="5" t="s">
         <v>269</v>
       </c>
@@ -5786,7 +5897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="5" t="s">
         <v>271</v>
       </c>
@@ -5797,7 +5908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="5" t="s">
         <v>273</v>
       </c>
@@ -5808,7 +5919,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="5" t="s">
         <v>276</v>
       </c>
@@ -5819,7 +5930,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="125.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="5" t="s">
         <v>62</v>
       </c>
@@ -5830,7 +5941,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="5" t="s">
         <v>64</v>
       </c>
@@ -5841,7 +5952,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="5" t="s">
         <v>66</v>
       </c>
@@ -5852,7 +5963,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="5" t="s">
         <v>68</v>
       </c>
@@ -5863,7 +5974,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="5" t="s">
         <v>72</v>
       </c>
@@ -5874,7 +5985,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="5" t="s">
         <v>280</v>
       </c>
@@ -5885,7 +5996,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="5" t="s">
         <v>74</v>
       </c>
@@ -5896,7 +6007,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="5" t="s">
         <v>283</v>
       </c>
@@ -5904,7 +6015,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="5" t="s">
         <v>285</v>
       </c>
@@ -5912,7 +6023,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="5" t="s">
         <v>287</v>
       </c>
@@ -5920,7 +6031,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="5" t="s">
         <v>289</v>
       </c>
@@ -5928,7 +6039,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="5" t="s">
         <v>290</v>
       </c>
@@ -5936,7 +6047,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="5" t="s">
         <v>291</v>
       </c>
@@ -5944,7 +6055,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="5" t="s">
         <v>80</v>
       </c>
@@ -5952,7 +6063,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="5" t="s">
         <v>82</v>
       </c>
@@ -5960,13 +6071,13 @@
         <v>222</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="4" t="s">
         <v>293</v>
       </c>
       <c r="B202" s="4"/>
     </row>
-    <row r="203" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="189.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="5" t="s">
         <v>294</v>
       </c>
@@ -5977,7 +6088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="7" t="s">
         <v>296</v>
       </c>
@@ -5988,7 +6099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="7" t="s">
         <v>232</v>
       </c>
@@ -5999,7 +6110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="7" t="s">
         <v>234</v>
       </c>
@@ -6010,7 +6121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="7" t="s">
         <v>236</v>
       </c>
@@ -6021,7 +6132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="7" t="s">
         <v>238</v>
       </c>
@@ -6032,7 +6143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="7" t="s">
         <v>240</v>
       </c>
@@ -6043,7 +6154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="7" t="s">
         <v>242</v>
       </c>
@@ -6054,7 +6165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="5" t="s">
         <v>244</v>
       </c>
@@ -6065,7 +6176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="7" t="s">
         <v>246</v>
       </c>
@@ -6076,7 +6187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="7" t="s">
         <v>299</v>
       </c>
@@ -6095,7 +6206,7 @@
       <c r="A215" s="5"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="5" t="s">
         <v>254</v>
       </c>
@@ -6106,7 +6217,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="5" t="s">
         <v>258</v>
       </c>
@@ -6117,7 +6228,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="5" t="s">
         <v>260</v>
       </c>
@@ -6128,7 +6239,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="5" t="s">
         <v>262</v>
       </c>
@@ -6139,7 +6250,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="5" t="s">
         <v>303</v>
       </c>
@@ -6150,7 +6261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="5" t="s">
         <v>305</v>
       </c>
@@ -6161,7 +6272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="5" t="s">
         <v>306</v>
       </c>
@@ -6172,7 +6283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="5" t="s">
         <v>307</v>
       </c>
@@ -6183,7 +6294,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="5" t="s">
         <v>309</v>
       </c>
@@ -6194,7 +6305,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="5" t="s">
         <v>64</v>
       </c>
@@ -6205,7 +6316,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="5" t="s">
         <v>66</v>
       </c>
@@ -6216,7 +6327,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="5" t="s">
         <v>68</v>
       </c>
@@ -6227,7 +6338,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="5" t="s">
         <v>72</v>
       </c>
@@ -6238,7 +6349,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="5" t="s">
         <v>280</v>
       </c>
@@ -6249,7 +6360,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="5" t="s">
         <v>74</v>
       </c>
@@ -6260,7 +6371,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="5" t="s">
         <v>80</v>
       </c>
@@ -6271,7 +6382,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="5" t="s">
         <v>82</v>
       </c>
@@ -6282,7 +6393,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="5" t="s">
         <v>313</v>
       </c>
@@ -6293,7 +6404,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="5" t="s">
         <v>315</v>
       </c>
@@ -6316,13 +6427,13 @@
       <c r="A237" s="5"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="4" t="s">
         <v>317</v>
       </c>
       <c r="B238" s="4"/>
     </row>
-    <row r="239" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="5" t="s">
         <v>318</v>
       </c>
@@ -6330,7 +6441,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="5" t="s">
         <v>320</v>
       </c>
@@ -6338,7 +6449,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="5" t="s">
         <v>36</v>
       </c>
@@ -6346,7 +6457,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="69.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="5" t="s">
         <v>38</v>
       </c>
@@ -6354,7 +6465,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="5" t="s">
         <v>324</v>
       </c>
@@ -6362,7 +6473,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="5" t="s">
         <v>325</v>
       </c>
@@ -6370,7 +6481,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="5" t="s">
         <v>149</v>
       </c>
@@ -6378,7 +6489,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="5" t="s">
         <v>151</v>
       </c>
@@ -6386,7 +6497,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="5" t="s">
         <v>328</v>
       </c>
@@ -6394,7 +6505,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="5" t="s">
         <v>330</v>
       </c>
@@ -6402,7 +6513,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="5" t="s">
         <v>332</v>
       </c>
@@ -6410,7 +6521,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="5" t="s">
         <v>334</v>
       </c>
@@ -6418,7 +6529,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="5" t="s">
         <v>336</v>
       </c>
@@ -6426,7 +6537,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="5" t="s">
         <v>338</v>
       </c>
@@ -6434,7 +6545,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="5" t="s">
         <v>339</v>
       </c>
@@ -6442,7 +6553,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="5" t="s">
         <v>341</v>
       </c>
@@ -6450,7 +6561,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="5" t="s">
         <v>343</v>
       </c>
@@ -6458,7 +6569,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="5" t="s">
         <v>344</v>
       </c>
@@ -6466,7 +6577,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="5" t="s">
         <v>346</v>
       </c>
@@ -6474,7 +6585,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="5" t="s">
         <v>348</v>
       </c>
@@ -6482,7 +6593,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="5" t="s">
         <v>350</v>
       </c>
@@ -6490,7 +6601,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="5" t="s">
         <v>352</v>
       </c>
@@ -6498,7 +6609,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="5" t="s">
         <v>353</v>
       </c>
@@ -6506,7 +6617,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="5" t="s">
         <v>355</v>
       </c>
@@ -6514,7 +6625,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="5" t="s">
         <v>356</v>
       </c>
@@ -6522,7 +6633,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="5" t="s">
         <v>358</v>
       </c>
@@ -6530,7 +6641,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="5" t="s">
         <v>359</v>
       </c>
@@ -6538,7 +6649,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="5" t="s">
         <v>360</v>
       </c>
@@ -6546,7 +6657,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="5" t="s">
         <v>361</v>
       </c>
@@ -6554,7 +6665,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="5" t="s">
         <v>363</v>
       </c>
@@ -6562,7 +6673,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="5" t="s">
         <v>364</v>
       </c>
@@ -6570,7 +6681,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="5" t="s">
         <v>62</v>
       </c>
@@ -6578,7 +6689,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="5" t="s">
         <v>64</v>
       </c>
@@ -6586,7 +6697,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="5" t="s">
         <v>66</v>
       </c>
@@ -6594,7 +6705,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="5" t="s">
         <v>68</v>
       </c>
@@ -6602,7 +6713,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="5" t="s">
         <v>72</v>
       </c>
@@ -6610,7 +6721,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="5" t="s">
         <v>366</v>
       </c>
@@ -6618,7 +6729,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="5" t="s">
         <v>74</v>
       </c>
@@ -6626,7 +6737,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="5" t="s">
         <v>80</v>
       </c>
@@ -6634,7 +6745,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="5" t="s">
         <v>82</v>
       </c>
@@ -6642,13 +6753,13 @@
         <v>312</v>
       </c>
     </row>
-    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="279" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="4" t="s">
         <v>368</v>
       </c>
       <c r="B279" s="4"/>
     </row>
-    <row r="280" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="170.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="5" t="s">
         <v>140</v>
       </c>
@@ -6656,7 +6767,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="5" t="s">
         <v>370</v>
       </c>
@@ -6664,7 +6775,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="5" t="s">
         <v>372</v>
       </c>
@@ -6672,7 +6783,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="5" t="s">
         <v>373</v>
       </c>
@@ -6680,7 +6791,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="5" t="s">
         <v>374</v>
       </c>
@@ -6688,7 +6799,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="5" t="s">
         <v>376</v>
       </c>
@@ -6696,7 +6807,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="5" t="s">
         <v>377</v>
       </c>
@@ -6704,7 +6815,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="5" t="s">
         <v>149</v>
       </c>
@@ -6712,7 +6823,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="5" t="s">
         <v>151</v>
       </c>
@@ -6720,7 +6831,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="5" t="s">
         <v>380</v>
       </c>
@@ -6728,7 +6839,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="5" t="s">
         <v>382</v>
       </c>
@@ -6736,7 +6847,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="5" t="s">
         <v>384</v>
       </c>
@@ -6744,7 +6855,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="5" t="s">
         <v>386</v>
       </c>
@@ -6752,7 +6863,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="5" t="s">
         <v>388</v>
       </c>
@@ -6760,7 +6871,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="5" t="s">
         <v>390</v>
       </c>
@@ -6768,7 +6879,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="5" t="s">
         <v>392</v>
       </c>
@@ -6776,7 +6887,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="5" t="s">
         <v>393</v>
       </c>
@@ -6784,7 +6895,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="5" t="s">
         <v>395</v>
       </c>
@@ -6792,7 +6903,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="5" t="s">
         <v>80</v>
       </c>
@@ -6800,7 +6911,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="5" t="s">
         <v>82</v>
       </c>
@@ -6808,13 +6919,13 @@
         <v>312</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="4" t="s">
         <v>397</v>
       </c>
       <c r="B300" s="4"/>
     </row>
-    <row r="301" customFormat="false" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="5" t="s">
         <v>398</v>
       </c>
@@ -6825,7 +6936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="5" t="s">
         <v>400</v>
       </c>
@@ -6836,7 +6947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="5" t="s">
         <v>402</v>
       </c>
@@ -6847,7 +6958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="5" t="s">
         <v>404</v>
       </c>
@@ -6858,7 +6969,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="92.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="93.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="5" t="s">
         <v>406</v>
       </c>
@@ -6869,7 +6980,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="5" t="s">
         <v>408</v>
       </c>
@@ -6880,7 +6991,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="307" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="5" t="s">
         <v>404</v>
       </c>
@@ -6891,13 +7002,13 @@
         <v>282</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="4" t="s">
         <v>410</v>
       </c>
       <c r="B308" s="4"/>
     </row>
-    <row r="309" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="5" t="s">
         <v>411</v>
       </c>
@@ -6905,7 +7016,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="36.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="36.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="5" t="s">
         <v>413</v>
       </c>
@@ -6913,7 +7024,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="5" t="s">
         <v>415</v>
       </c>
@@ -6921,7 +7032,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="5" t="s">
         <v>417</v>
       </c>
@@ -6929,7 +7040,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="5" t="s">
         <v>419</v>
       </c>
@@ -6937,7 +7048,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="5" t="s">
         <v>420</v>
       </c>
@@ -6945,7 +7056,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="315" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="5" t="s">
         <v>422</v>
       </c>
@@ -6953,7 +7064,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="5" t="s">
         <v>424</v>
       </c>
@@ -6961,7 +7072,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="5" t="s">
         <v>426</v>
       </c>
@@ -6969,7 +7080,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="5" t="s">
         <v>428</v>
       </c>
@@ -6977,7 +7088,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="5" t="s">
         <v>430</v>
       </c>
@@ -6985,7 +7096,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="5" t="s">
         <v>432</v>
       </c>
@@ -6993,7 +7104,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="5" t="s">
         <v>434</v>
       </c>
@@ -7001,7 +7112,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="5" t="s">
         <v>436</v>
       </c>
@@ -7009,7 +7120,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="5" t="s">
         <v>438</v>
       </c>
@@ -7017,7 +7128,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="5" t="s">
         <v>440</v>
       </c>
@@ -7025,7 +7136,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="5" t="s">
         <v>442</v>
       </c>
@@ -7033,7 +7144,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="38.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="5" t="s">
         <v>444</v>
       </c>
@@ -7041,7 +7152,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="38.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="5" t="s">
         <v>446</v>
       </c>
@@ -7049,7 +7160,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="5" t="s">
         <v>448</v>
       </c>
@@ -7057,7 +7168,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="5" t="s">
         <v>450</v>
       </c>
@@ -7065,7 +7176,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="5" t="s">
         <v>452</v>
       </c>
@@ -7073,7 +7184,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="159.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="5" t="s">
         <v>454</v>
       </c>
@@ -7081,7 +7192,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="332" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="5" t="s">
         <v>64</v>
       </c>
@@ -7089,7 +7200,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="5" t="s">
         <v>66</v>
       </c>
@@ -7097,7 +7208,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="334" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="5" t="s">
         <v>68</v>
       </c>
@@ -7105,7 +7216,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="5" t="s">
         <v>72</v>
       </c>
@@ -7113,7 +7224,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="5" t="s">
         <v>366</v>
       </c>
@@ -7121,7 +7232,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="337" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="5" t="s">
         <v>74</v>
       </c>
@@ -7129,7 +7240,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="5" t="s">
         <v>456</v>
       </c>
@@ -7137,7 +7248,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="5" t="s">
         <v>458</v>
       </c>
@@ -7145,7 +7256,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="5" t="s">
         <v>460</v>
       </c>
@@ -7157,13 +7268,13 @@
       <c r="A341" s="5"/>
       <c r="B341" s="5"/>
     </row>
-    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="2" t="s">
         <v>462</v>
       </c>
       <c r="B342" s="3"/>
     </row>
-    <row r="343" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="5" t="s">
         <v>463</v>
       </c>
@@ -7171,7 +7282,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="5" t="s">
         <v>465</v>
       </c>
@@ -7179,7 +7290,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="5" t="s">
         <v>467</v>
       </c>
@@ -7187,7 +7298,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="5" t="s">
         <v>469</v>
       </c>
@@ -7195,7 +7306,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="5" t="s">
         <v>471</v>
       </c>
@@ -7203,7 +7314,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="5" t="s">
         <v>473</v>
       </c>
@@ -7211,7 +7322,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="5" t="s">
         <v>475</v>
       </c>
@@ -7219,7 +7330,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="5" t="s">
         <v>477</v>
       </c>

</xml_diff>

<commit_message>
Fixed PluginUsers page tests.
</commit_message>
<xml_diff>
--- a/Domibus-MSH-selenium-ui-tests/TestCase_Domibus-4.1.xlsx
+++ b/Domibus-MSH-selenium-ui-tests/TestCase_Domibus-4.1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="800">
   <si>
     <t xml:space="preserve">Step</t>
   </si>
@@ -823,6 +823,9 @@
 (repeat for each filter and for multiple combinations of filters)</t>
   </si>
   <si>
+    <t xml:space="preserve">lp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Delete message</t>
   </si>
   <si>
@@ -835,37 +838,8 @@
     <t xml:space="preserve">Move message</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Modal with </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">possible</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> destinations opens allowing the user to cancel or confirm the action
+    <t xml:space="preserve">Modal with possible destinations opens allowing the user to cancel or confirm the action
 If the user confirms the message is moved to the selected destination queue. Else the message is not moved</t>
-    </r>
   </si>
   <si>
     <r>
@@ -991,9 +965,6 @@
   </si>
   <si>
     <t xml:space="preserve">List is downloaded and corresponds to the active domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lp</t>
   </si>
   <si>
     <t xml:space="preserve">Upload random file</t>
@@ -4105,8 +4076,8 @@
   </sheetPr>
   <dimension ref="A1:D351"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A334" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B348" activeCellId="0" sqref="B348"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C115" activeCellId="0" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4173,7 +4144,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -4213,7 +4184,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -4289,7 +4260,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="216.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -4313,7 +4284,7 @@
       </c>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
@@ -4327,7 +4298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
@@ -4363,7 +4334,7 @@
       </c>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
@@ -4435,7 +4406,7 @@
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="75.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="75.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
         <v>47</v>
       </c>
@@ -4459,7 +4430,7 @@
       </c>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
         <v>51</v>
       </c>
@@ -4471,7 +4442,7 @@
       </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>53</v>
       </c>
@@ -4523,7 +4494,7 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="323.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="324.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
         <v>62</v>
       </c>
@@ -4533,7 +4504,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
         <v>64</v>
       </c>
@@ -4553,7 +4524,7 @@
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
         <v>68</v>
       </c>
@@ -4573,7 +4544,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
         <v>72</v>
       </c>
@@ -4603,7 +4574,7 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
         <v>78</v>
       </c>
@@ -4653,7 +4624,7 @@
       </c>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
         <v>87</v>
       </c>
@@ -4665,7 +4636,7 @@
       </c>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
         <v>89</v>
       </c>
@@ -4737,7 +4708,7 @@
       </c>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
         <v>100</v>
       </c>
@@ -4749,7 +4720,7 @@
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="82.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
         <v>102</v>
       </c>
@@ -4843,7 +4814,7 @@
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
         <v>116</v>
       </c>
@@ -4883,7 +4854,7 @@
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
     </row>
-    <row r="71" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
         <v>124</v>
       </c>
@@ -4913,7 +4884,7 @@
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
     </row>
-    <row r="74" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
         <v>130</v>
       </c>
@@ -4923,7 +4894,7 @@
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
     </row>
-    <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
         <v>132</v>
       </c>
@@ -4933,7 +4904,7 @@
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
     </row>
-    <row r="76" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>133</v>
       </c>
@@ -4991,7 +4962,7 @@
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
     </row>
-    <row r="82" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="136.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
         <v>140</v>
       </c>
@@ -5013,7 +4984,7 @@
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
     </row>
-    <row r="84" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
         <v>144</v>
       </c>
@@ -5085,7 +5056,7 @@
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
     </row>
-    <row r="91" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="136.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
         <v>62</v>
       </c>
@@ -5095,7 +5066,7 @@
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
     </row>
-    <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
         <v>64</v>
       </c>
@@ -5115,7 +5086,7 @@
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
     </row>
-    <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
         <v>68</v>
       </c>
@@ -5135,7 +5106,7 @@
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
     </row>
-    <row r="96" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
         <v>72</v>
       </c>
@@ -5185,7 +5156,7 @@
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
     </row>
-    <row r="101" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
         <v>164</v>
       </c>
@@ -5211,7 +5182,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
         <v>170</v>
       </c>
@@ -5248,6 +5219,9 @@
       <c r="B108" s="5" t="s">
         <v>174</v>
       </c>
+      <c r="C108" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
@@ -5256,13 +5230,19 @@
       <c r="B109" s="5" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="110" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C109" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
         <v>176</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>37</v>
+      </c>
+      <c r="C110" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5272,6 +5252,9 @@
       <c r="B111" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="C111" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
@@ -5280,6 +5263,9 @@
       <c r="B112" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="C112" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
@@ -5288,24 +5274,30 @@
       <c r="B113" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="114" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D113" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="82.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>179</v>
+      </c>
+      <c r="C114" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B115" s="7" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
         <v>51</v>
       </c>
@@ -5317,7 +5309,7 @@
       <c r="A117" s="5"/>
       <c r="B117" s="5"/>
     </row>
-    <row r="118" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
         <v>53</v>
       </c>
@@ -5325,20 +5317,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5349,15 +5341,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="136.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
         <v>64</v>
       </c>
@@ -5373,23 +5365,23 @@
         <v>67</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
         <v>72</v>
       </c>
@@ -5402,7 +5394,7 @@
         <v>74</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5410,63 +5402,63 @@
         <v>159</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B135" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5491,16 +5483,16 @@
     </row>
     <row r="140" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B140" s="4"/>
     </row>
     <row r="141" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C141" s="1" t="n">
         <v>1</v>
@@ -5508,10 +5500,10 @@
     </row>
     <row r="142" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>1</v>
@@ -5519,13 +5511,13 @@
     </row>
     <row r="143" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5536,7 +5528,7 @@
         <v>210</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5547,10 +5539,10 @@
         <v>212</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="109.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="s">
         <v>62</v>
       </c>
@@ -5558,10 +5550,10 @@
         <v>213</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="5" t="s">
         <v>64</v>
       </c>
@@ -5569,7 +5561,7 @@
         <v>65</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5580,21 +5572,21 @@
         <v>67</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="5" t="s">
         <v>72</v>
       </c>
@@ -5602,7 +5594,7 @@
         <v>73</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5613,7 +5605,7 @@
         <v>214</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5638,7 +5630,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="s">
         <v>220</v>
       </c>
@@ -5668,7 +5660,7 @@
         <v>81</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5679,7 +5671,7 @@
         <v>224</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5732,7 +5724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="8" t="s">
         <v>234</v>
       </c>
@@ -5743,7 +5735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="8" t="s">
         <v>236</v>
       </c>
@@ -5765,7 +5757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="8" t="s">
         <v>240</v>
       </c>
@@ -5776,7 +5768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="8" t="s">
         <v>242</v>
       </c>
@@ -5787,7 +5779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="8" t="s">
         <v>244</v>
       </c>
@@ -5798,7 +5790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="5" t="s">
         <v>246</v>
       </c>
@@ -5820,7 +5812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="8" t="s">
         <v>250</v>
       </c>
@@ -5875,7 +5867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="5" t="s">
         <v>260</v>
       </c>
@@ -5908,7 +5900,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="5" t="s">
         <v>266</v>
       </c>
@@ -5941,7 +5933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="5" t="s">
         <v>270</v>
       </c>
@@ -5952,7 +5944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="5" t="s">
         <v>271</v>
       </c>
@@ -5974,7 +5966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="5" t="s">
         <v>275</v>
       </c>
@@ -5985,7 +5977,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="5" t="s">
         <v>278</v>
       </c>
@@ -6007,7 +5999,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="5" t="s">
         <v>64</v>
       </c>
@@ -6029,7 +6021,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="5" t="s">
         <v>68</v>
       </c>
@@ -6040,7 +6032,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="5" t="s">
         <v>72</v>
       </c>
@@ -6105,7 +6097,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="5" t="s">
         <v>292</v>
       </c>
@@ -6143,7 +6135,7 @@
       </c>
       <c r="B202" s="4"/>
     </row>
-    <row r="203" customFormat="false" ht="188.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="189.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="5" t="s">
         <v>296</v>
       </c>
@@ -6165,7 +6157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="8" t="s">
         <v>234</v>
       </c>
@@ -6176,7 +6168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="8" t="s">
         <v>236</v>
       </c>
@@ -6198,7 +6190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="8" t="s">
         <v>240</v>
       </c>
@@ -6209,7 +6201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="8" t="s">
         <v>242</v>
       </c>
@@ -6220,7 +6212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="8" t="s">
         <v>244</v>
       </c>
@@ -6231,7 +6223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="44.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="5" t="s">
         <v>246</v>
       </c>
@@ -6283,7 +6275,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="5" t="s">
         <v>260</v>
       </c>
@@ -6327,7 +6319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="5" t="s">
         <v>307</v>
       </c>
@@ -6338,7 +6330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="5" t="s">
         <v>308</v>
       </c>
@@ -6349,7 +6341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="109.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="5" t="s">
         <v>309</v>
       </c>
@@ -6371,7 +6363,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="5" t="s">
         <v>64</v>
       </c>
@@ -6393,7 +6385,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="5" t="s">
         <v>68</v>
       </c>
@@ -6404,7 +6396,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="5" t="s">
         <v>72</v>
       </c>
@@ -6448,7 +6440,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="5" t="s">
         <v>82</v>
       </c>
@@ -6515,7 +6507,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="5" t="s">
         <v>36</v>
       </c>
@@ -6523,7 +6515,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="82.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="5" t="s">
         <v>38</v>
       </c>
@@ -6587,7 +6579,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="5" t="s">
         <v>336</v>
       </c>
@@ -6595,7 +6587,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="5" t="s">
         <v>338</v>
       </c>
@@ -6611,7 +6603,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="5" t="s">
         <v>341</v>
       </c>
@@ -6619,7 +6611,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="5" t="s">
         <v>343</v>
       </c>
@@ -6627,7 +6619,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="255" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="5" t="s">
         <v>345</v>
       </c>
@@ -6747,7 +6739,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="109.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="5" t="s">
         <v>62</v>
       </c>
@@ -6755,7 +6747,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="271" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="5" t="s">
         <v>64</v>
       </c>
@@ -6771,7 +6763,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="5" t="s">
         <v>68</v>
       </c>
@@ -6779,7 +6771,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="5" t="s">
         <v>72</v>
       </c>
@@ -6811,7 +6803,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="5" t="s">
         <v>82</v>
       </c>
@@ -6857,7 +6849,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="5" t="s">
         <v>376</v>
       </c>
@@ -6905,7 +6897,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="5" t="s">
         <v>384</v>
       </c>
@@ -6921,7 +6913,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="292" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="5" t="s">
         <v>388</v>
       </c>
@@ -6961,7 +6953,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="5" t="s">
         <v>397</v>
       </c>
@@ -6977,7 +6969,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="5" t="s">
         <v>82</v>
       </c>
@@ -6991,7 +6983,7 @@
       </c>
       <c r="B300" s="4"/>
     </row>
-    <row r="301" customFormat="false" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="5" t="s">
         <v>400</v>
       </c>
@@ -7002,7 +6994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="5" t="s">
         <v>402</v>
       </c>
@@ -7035,7 +7027,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="92.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="93.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="5" t="s">
         <v>408</v>
       </c>
@@ -7074,7 +7066,7 @@
       </c>
       <c r="B308" s="4"/>
     </row>
-    <row r="309" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="5" t="s">
         <v>413</v>
       </c>
@@ -7085,7 +7077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="5" t="s">
         <v>415</v>
       </c>
@@ -7093,7 +7085,7 @@
         <v>416</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7104,7 +7096,7 @@
         <v>418</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7115,7 +7107,7 @@
         <v>420</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7129,7 +7121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="27.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="5" t="s">
         <v>422</v>
       </c>
@@ -7148,7 +7140,7 @@
         <v>425</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7159,7 +7151,7 @@
         <v>427</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7170,7 +7162,7 @@
         <v>429</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7181,7 +7173,7 @@
         <v>431</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7192,7 +7184,7 @@
         <v>433</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7203,10 +7195,10 @@
         <v>435</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="321" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="5" t="s">
         <v>436</v>
       </c>
@@ -7236,7 +7228,7 @@
         <v>441</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7261,7 +7253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" customFormat="false" ht="38.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="5" t="s">
         <v>446</v>
       </c>
@@ -7272,7 +7264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="38.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="38.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="5" t="s">
         <v>448</v>
       </c>
@@ -7316,7 +7308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="190" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="5" t="s">
         <v>456</v>
       </c>
@@ -7324,10 +7316,10 @@
         <v>457</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="332" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="5" t="s">
         <v>64</v>
       </c>
@@ -7335,7 +7327,7 @@
         <v>65</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7346,10 +7338,10 @@
         <v>67</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="334" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="5" t="s">
         <v>68</v>
       </c>
@@ -7357,10 +7349,10 @@
         <v>280</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="335" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="5" t="s">
         <v>72</v>
       </c>
@@ -7368,7 +7360,7 @@
         <v>281</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7379,7 +7371,7 @@
         <v>369</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7401,7 +7393,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="339" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="5" t="s">
         <v>460</v>
       </c>
@@ -7433,7 +7425,7 @@
       </c>
       <c r="B342" s="3"/>
     </row>
-    <row r="343" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" customFormat="false" ht="55.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="5" t="s">
         <v>465</v>
       </c>
@@ -7465,7 +7457,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="5" t="s">
         <v>473</v>
       </c>
@@ -7481,7 +7473,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="5" t="s">
         <v>477</v>
       </c>
@@ -7489,7 +7481,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="28.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="5" t="s">
         <v>479</v>
       </c>

</xml_diff>

<commit_message>
Minor fixes for some tests (1).
</commit_message>
<xml_diff>
--- a/Domibus-MSH-selenium-ui-tests/TestCase_Domibus-4.1.xlsx
+++ b/Domibus-MSH-selenium-ui-tests/TestCase_Domibus-4.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" state="visible" r:id="rId2"/>
@@ -2992,7 +2992,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3182,8 +3182,8 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3360,8 +3360,8 @@
   </sheetPr>
   <dimension ref="A1:D354"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A341" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D355" activeCellId="0" sqref="D355"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D107" activeCellId="0" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7572,6 +7572,7 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Minor changes to wait times and wait behaviour
</commit_message>
<xml_diff>
--- a/Domibus-MSH-selenium-ui-tests/TestCase_Domibus-4.1.xlsx
+++ b/Domibus-MSH-selenium-ui-tests/TestCase_Domibus-4.1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="511">
   <si>
     <t xml:space="preserve">TEST AUTOMATION STATUS REPORT</t>
   </si>
@@ -3276,11 +3276,11 @@
       </c>
       <c r="B8" s="6" t="n">
         <f aca="false">COUNTIF('RegressionScenarios-4.1'!D1:D500,"="&amp;A8)</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="8" t="n">
         <f aca="false">B8/B$6</f>
-        <v>0.172727272727273</v>
+        <v>0.16969696969697</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3361,7 +3361,7 @@
   <dimension ref="A1:D354"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D107" activeCellId="0" sqref="D107"/>
+      <selection pane="topLeft" activeCell="C108" activeCellId="0" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4621,10 +4621,10 @@
       <c r="B107" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C107" s="16"/>
-      <c r="D107" s="12" t="s">
-        <v>74</v>
-      </c>
+      <c r="C107" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D107" s="12"/>
     </row>
     <row r="108" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="12" t="s">

</xml_diff>